<commit_message>
Added multiple test data to excel and validate
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata_cdcalculator.xlsx
+++ b/src/main/resources/testdata_cdcalculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Automation\automate-citbank-cd-calculator\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6490E7E-8F14-409D-850E-FCD62F1D409E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469259A3-BA69-4498-A9EB-E50BFB8C7DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7069F9CF-838F-47F3-875D-916362C89D4D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>InitialDeposit</t>
   </si>
@@ -52,6 +52,66 @@
   </si>
   <si>
     <t>01.60</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Short-term CD</t>
+  </si>
+  <si>
+    <t>Medium term</t>
+  </si>
+  <si>
+    <t>Large principal</t>
+  </si>
+  <si>
+    <t>Low deposit</t>
+  </si>
+  <si>
+    <t>Minimum edge case</t>
+  </si>
+  <si>
+    <t>Max edge case</t>
+  </si>
+  <si>
+    <t>Zero months</t>
+  </si>
+  <si>
+    <t>Negative term</t>
+  </si>
+  <si>
+    <t>Zero interest</t>
+  </si>
+  <si>
+    <t>Negative interest</t>
+  </si>
+  <si>
+    <t>Zero deposit</t>
+  </si>
+  <si>
+    <t>02.00</t>
+  </si>
+  <si>
+    <t>01.80</t>
+  </si>
+  <si>
+    <t>02.50</t>
+  </si>
+  <si>
+    <t>01.40</t>
+  </si>
+  <si>
+    <t>05.00</t>
+  </si>
+  <si>
+    <t>-01.00</t>
+  </si>
+  <si>
+    <t>00.01</t>
   </si>
 </sst>
 </file>
@@ -59,7 +119,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="[$$-1009]#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$$-1009]#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -78,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,6 +149,11 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
       </patternFill>
     </fill>
   </fills>
@@ -104,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -119,13 +184,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4669D5-9AD2-473B-A8EA-5D8F530CC8C4}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -454,9 +520,10 @@
     <col min="4" max="4" width="24.36328125" customWidth="1"/>
     <col min="5" max="5" width="16.90625" style="8" customWidth="1"/>
     <col min="6" max="6" width="25.453125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -475,8 +542,11 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>31500</v>
       </c>
@@ -494,6 +564,262 @@
       </c>
       <c r="F2" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="7">
+        <v>51010.04</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>25000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>24</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="7">
+        <v>25916.37</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>60</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="7">
+        <v>113314.36</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>15000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>36</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="7">
+        <v>15643.4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>9999999</v>
+      </c>
+      <c r="B8" s="1">
+        <v>120</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="7">
+        <v>16486646.49</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="7">
+        <v>16486646.49</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>-12</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="7">
+        <v>30483.85</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B11" s="1">
+        <v>12</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="7">
+        <v>30483.85</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>12</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="7">
+        <v>30301.5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="7">
+        <v>30301.5</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add test data file and code to fetch them
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata_cdcalculator.xlsx
+++ b/src/main/resources/testdata_cdcalculator.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Automation\automate-citbank-cd-calculator\src\main\resources\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
   <si>
     <t>InitialDeposit</t>
   </si>
@@ -138,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +156,11 @@
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -169,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -192,6 +197,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,13 +531,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" customWidth="1"/>
-    <col min="3" max="3" width="17.6328125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="24.36328125" customWidth="1"/>
-    <col min="5" max="5" width="16.90625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.453125" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.54296875"/>
+    <col min="2" max="2" customWidth="true" width="15.54296875"/>
+    <col min="3" max="3" customWidth="true" style="4" width="17.6328125"/>
+    <col min="4" max="4" customWidth="true" width="24.36328125"/>
+    <col min="5" max="5" customWidth="true" style="8" width="16.90625"/>
+    <col min="6" max="6" customWidth="true" width="25.453125"/>
+    <col min="7" max="7" customWidth="true" width="12.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -565,7 +582,7 @@
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -588,7 +605,7 @@
       <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -611,7 +628,7 @@
       <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="12" t="s">
         <v>10</v>
       </c>
     </row>
@@ -634,7 +651,7 @@
       <c r="F5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="13" t="s">
         <v>10</v>
       </c>
     </row>
@@ -657,7 +674,7 @@
       <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -680,7 +697,7 @@
       <c r="F7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="15" t="s">
         <v>10</v>
       </c>
     </row>
@@ -703,7 +720,7 @@
       <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="16" t="s">
         <v>10</v>
       </c>
     </row>
@@ -726,7 +743,7 @@
       <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="17" t="s">
         <v>10</v>
       </c>
     </row>
@@ -749,7 +766,7 @@
       <c r="F10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -772,7 +789,7 @@
       <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="19" t="s">
         <v>10</v>
       </c>
     </row>
@@ -795,7 +812,7 @@
       <c r="F12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="20" t="s">
         <v>10</v>
       </c>
     </row>
@@ -818,7 +835,7 @@
       <c r="F13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="21" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new test method & parallel testing, serial testing
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata_cdcalculator.xlsx
+++ b/src/main/resources/testdata_cdcalculator.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Automation\automate-citbank-cd-calculator\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469259A3-BA69-4498-A9EB-E50BFB8C7DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06406810-1DA1-4420-85AD-E9D18F8B0FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7069F9CF-838F-47F3-875D-916362C89D4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Compounded_Daily" sheetId="1" r:id="rId1"/>
+    <sheet name="Compounded_Monthly" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="33">
   <si>
     <t>InitialDeposit</t>
   </si>
@@ -54,9 +55,6 @@
     <t>01.60</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Passed</t>
   </si>
   <si>
@@ -112,6 +110,21 @@
   </si>
   <si>
     <t>00.01</t>
+  </si>
+  <si>
+    <t>Compounded Monthly</t>
+  </si>
+  <si>
+    <t>Status Chrome</t>
+  </si>
+  <si>
+    <t>Status edge</t>
+  </si>
+  <si>
+    <t>Status chrome</t>
+  </si>
+  <si>
+    <t>Status firefox</t>
   </si>
 </sst>
 </file>
@@ -138,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,11 +169,6 @@
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -174,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -197,18 +205,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4669D5-9AD2-473B-A8EA-5D8F530CC8C4}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
@@ -531,16 +527,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.54296875"/>
-    <col min="2" max="2" customWidth="true" width="15.54296875"/>
-    <col min="3" max="3" customWidth="true" style="4" width="17.6328125"/>
-    <col min="4" max="4" customWidth="true" width="24.36328125"/>
-    <col min="5" max="5" customWidth="true" style="8" width="16.90625"/>
-    <col min="6" max="6" customWidth="true" width="25.453125"/>
-    <col min="7" max="7" customWidth="true" width="12.0"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" customWidth="1"/>
+    <col min="3" max="3" width="17.6328125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.36328125" customWidth="1"/>
+    <col min="5" max="5" width="16.90625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" customWidth="1"/>
+    <col min="8" max="8" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -560,10 +557,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>31500</v>
       </c>
@@ -582,11 +582,14 @@
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>50000</v>
       </c>
@@ -594,7 +597,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -603,13 +606,16 @@
         <v>51010.04</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>25000</v>
       </c>
@@ -617,7 +623,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -626,13 +632,16 @@
         <v>25916.37</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>100000</v>
       </c>
@@ -640,7 +649,7 @@
         <v>60</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -649,13 +658,16 @@
         <v>113314.36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>15000</v>
       </c>
@@ -663,7 +675,7 @@
         <v>36</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
@@ -672,13 +684,16 @@
         <v>15643.4</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -686,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>6</v>
@@ -695,13 +710,16 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>9999999</v>
       </c>
@@ -709,7 +727,7 @@
         <v>120</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>6</v>
@@ -718,13 +736,16 @@
         <v>16486646.49</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>30000</v>
       </c>
@@ -741,13 +762,16 @@
         <v>16486646.49</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>30000</v>
       </c>
@@ -764,13 +788,16 @@
         <v>30483.85</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>30000</v>
       </c>
@@ -787,13 +814,16 @@
         <v>30483.85</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>30000</v>
       </c>
@@ -801,7 +831,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>6</v>
@@ -810,13 +840,16 @@
         <v>30301.5</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -824,7 +857,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
@@ -833,14 +866,380 @@
         <v>30301.5</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CE2FBF-79F0-461C-8A13-1762CE45C5DB}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.90625" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.6328125" customWidth="1"/>
+    <col min="4" max="4" width="24.08984375" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" customWidth="1"/>
+    <col min="7" max="7" width="14.81640625" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>31500</v>
+      </c>
+      <c r="B2" s="1">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="7">
+        <v>32050.75</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="7">
+        <v>51010.04</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>25000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>24</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="7">
+        <v>25916.37</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>60</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="7">
+        <v>113314.36</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>15000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>36</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="7">
+        <v>15643.4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>9999999</v>
+      </c>
+      <c r="B8" s="1">
+        <v>120</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="7">
+        <v>16486646.49</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="7">
+        <v>16486646.49</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>-12</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="7">
+        <v>30483.85</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B11" s="1">
+        <v>12</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="7">
+        <v>30483.85</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>12</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="7">
+        <v>30301.5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="7">
+        <v>30301.5</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding listners in our projects, serial and parallel testing accrosss multiple browsers
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata_cdcalculator.xlsx
+++ b/src/main/resources/testdata_cdcalculator.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Automation\automate-citbank-cd-calculator\src\main\resources\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="33">
   <si>
     <t>InitialDeposit</t>
   </si>
@@ -151,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +169,11 @@
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -182,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -205,6 +210,78 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,14 +604,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" customWidth="1"/>
-    <col min="3" max="3" width="17.6328125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="24.36328125" customWidth="1"/>
-    <col min="5" max="5" width="16.90625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.453125" customWidth="1"/>
-    <col min="7" max="7" width="15.7265625" customWidth="1"/>
-    <col min="8" max="8" width="15.6328125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.54296875"/>
+    <col min="2" max="2" customWidth="true" width="15.54296875"/>
+    <col min="3" max="3" customWidth="true" style="4" width="17.6328125"/>
+    <col min="4" max="4" customWidth="true" width="24.36328125"/>
+    <col min="5" max="5" customWidth="true" style="8" width="16.90625"/>
+    <col min="6" max="6" customWidth="true" width="25.453125"/>
+    <col min="7" max="7" customWidth="true" width="15.7265625"/>
+    <col min="8" max="8" customWidth="true" width="15.6328125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -582,7 +659,7 @@
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="70" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="9" t="s">
@@ -608,7 +685,7 @@
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="71" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -634,7 +711,7 @@
       <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="72" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="9" t="s">
@@ -660,7 +737,7 @@
       <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="73" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="9" t="s">
@@ -686,7 +763,7 @@
       <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="74" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="9" t="s">
@@ -712,7 +789,7 @@
       <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="75" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -738,7 +815,7 @@
       <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="76" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="9" t="s">
@@ -764,7 +841,7 @@
       <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="77" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="9" t="s">
@@ -790,7 +867,7 @@
       <c r="F10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="78" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="9" t="s">
@@ -816,7 +893,7 @@
       <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="79" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -842,7 +919,7 @@
       <c r="F12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="80" t="s">
         <v>9</v>
       </c>
       <c r="H12" s="9" t="s">
@@ -868,7 +945,7 @@
       <c r="F13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="81" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="9" t="s">
@@ -891,14 +968,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.90625" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" customWidth="1"/>
-    <col min="3" max="3" width="18.6328125" customWidth="1"/>
-    <col min="4" max="4" width="24.08984375" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="17.6328125" customWidth="1"/>
-    <col min="7" max="7" width="14.81640625" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.90625"/>
+    <col min="2" max="2" customWidth="true" width="15.453125"/>
+    <col min="3" max="3" customWidth="true" width="18.6328125"/>
+    <col min="4" max="4" customWidth="true" width="24.08984375"/>
+    <col min="5" max="5" customWidth="true" width="17.0"/>
+    <col min="6" max="6" customWidth="true" width="17.6328125"/>
+    <col min="7" max="7" customWidth="true" width="14.81640625"/>
+    <col min="8" max="8" customWidth="true" width="13.81640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added page object model in project by creating package pages and implement those method in test classes
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata_cdcalculator.xlsx
+++ b/src/main/resources/testdata_cdcalculator.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="34">
   <si>
     <t>InitialDeposit</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Status firefox</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -151,7 +154,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +177,16 @@
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -187,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -282,6 +295,90 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,7 +756,7 @@
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="70" t="s">
+      <c r="G2" s="142" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="9" t="s">
@@ -685,7 +782,7 @@
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="143" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -711,7 +808,7 @@
       <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="72" t="s">
+      <c r="G4" s="144" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="9" t="s">
@@ -737,7 +834,7 @@
       <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="145" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="9" t="s">
@@ -763,7 +860,7 @@
       <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="74" t="s">
+      <c r="G6" s="146" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="9" t="s">
@@ -789,7 +886,7 @@
       <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="75" t="s">
+      <c r="G7" s="147" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -815,7 +912,7 @@
       <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="76" t="s">
+      <c r="G8" s="148" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="9" t="s">
@@ -841,7 +938,7 @@
       <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="77" t="s">
+      <c r="G9" s="149" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="9" t="s">
@@ -867,7 +964,7 @@
       <c r="F10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="78" t="s">
+      <c r="G10" s="150" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="9" t="s">
@@ -893,7 +990,7 @@
       <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="79" t="s">
+      <c r="G11" s="151" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -919,7 +1016,7 @@
       <c r="F12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="80" t="s">
+      <c r="G12" s="152" t="s">
         <v>9</v>
       </c>
       <c r="H12" s="9" t="s">
@@ -945,7 +1042,7 @@
       <c r="F13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="81" t="s">
+      <c r="G13" s="153" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="9" t="s">
@@ -1026,8 +1123,8 @@
       <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>9</v>
+      <c r="H2" s="154" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1052,8 +1149,8 @@
       <c r="G3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>9</v>
+      <c r="H3" s="155" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -1078,8 +1175,8 @@
       <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>9</v>
+      <c r="H4" s="156" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -1104,8 +1201,8 @@
       <c r="G5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>9</v>
+      <c r="H5" s="157" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -1130,8 +1227,8 @@
       <c r="G6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>9</v>
+      <c r="H6" s="158" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1156,7 +1253,7 @@
       <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="159" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1182,8 +1279,8 @@
       <c r="G8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>9</v>
+      <c r="H8" s="160" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -1208,8 +1305,8 @@
       <c r="G9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>9</v>
+      <c r="H9" s="161" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1234,8 +1331,8 @@
       <c r="G10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>9</v>
+      <c r="H10" s="162" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1260,8 +1357,8 @@
       <c r="G11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="9" t="s">
-        <v>9</v>
+      <c r="H11" s="163" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1286,8 +1383,8 @@
       <c r="G12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>9</v>
+      <c r="H12" s="164" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1312,8 +1409,8 @@
       <c r="G13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="9" t="s">
-        <v>9</v>
+      <c r="H13" s="165" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added extent report with lister in project
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata_cdcalculator.xlsx
+++ b/src/main/resources/testdata_cdcalculator.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="34">
   <si>
     <t>InitialDeposit</t>
   </si>
@@ -200,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="298">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -379,6 +379,138 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,7 +888,7 @@
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="142" t="s">
+      <c r="G2" s="286" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="9" t="s">
@@ -782,7 +914,7 @@
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="143" t="s">
+      <c r="G3" s="287" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -808,7 +940,7 @@
       <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="144" t="s">
+      <c r="G4" s="288" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="9" t="s">
@@ -834,7 +966,7 @@
       <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="145" t="s">
+      <c r="G5" s="289" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="9" t="s">
@@ -860,7 +992,7 @@
       <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="146" t="s">
+      <c r="G6" s="290" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="9" t="s">
@@ -886,7 +1018,7 @@
       <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="147" t="s">
+      <c r="G7" s="291" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -912,7 +1044,7 @@
       <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="148" t="s">
+      <c r="G8" s="292" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="9" t="s">
@@ -938,7 +1070,7 @@
       <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="149" t="s">
+      <c r="G9" s="293" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="9" t="s">
@@ -964,7 +1096,7 @@
       <c r="F10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="150" t="s">
+      <c r="G10" s="294" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="9" t="s">
@@ -990,7 +1122,7 @@
       <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="151" t="s">
+      <c r="G11" s="295" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -1016,7 +1148,7 @@
       <c r="F12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="152" t="s">
+      <c r="G12" s="296" t="s">
         <v>9</v>
       </c>
       <c r="H12" s="9" t="s">
@@ -1042,7 +1174,7 @@
       <c r="F13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="153" t="s">
+      <c r="G13" s="297" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="9" t="s">
@@ -1123,7 +1255,7 @@
       <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="154" t="s">
+      <c r="H2" s="274" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1149,7 +1281,7 @@
       <c r="G3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="155" t="s">
+      <c r="H3" s="275" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1175,7 +1307,7 @@
       <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="156" t="s">
+      <c r="H4" s="276" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1201,7 +1333,7 @@
       <c r="G5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="157" t="s">
+      <c r="H5" s="277" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1227,7 +1359,7 @@
       <c r="G6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="158" t="s">
+      <c r="H6" s="278" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1253,7 +1385,7 @@
       <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="159" t="s">
+      <c r="H7" s="279" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1279,7 +1411,7 @@
       <c r="G8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="160" t="s">
+      <c r="H8" s="280" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1305,7 +1437,7 @@
       <c r="G9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="161" t="s">
+      <c r="H9" s="281" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1331,7 +1463,7 @@
       <c r="G10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="162" t="s">
+      <c r="H10" s="282" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1357,7 +1489,7 @@
       <c r="G11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="163" t="s">
+      <c r="H11" s="283" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1383,7 +1515,7 @@
       <c r="G12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="164" t="s">
+      <c r="H12" s="284" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1409,7 +1541,7 @@
       <c r="G13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="165" t="s">
+      <c r="H13" s="285" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>